<commit_message>
Added hardening to weak-plane shear.  Fixes #3565
</commit_message>
<xml_diff>
--- a/modules/tensor_mechanics/tests/weak_plane_shear/small_deform2.xlsx
+++ b/modules/tensor_mechanics/tests/weak_plane_shear/small_deform2.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="72" windowWidth="15300" windowHeight="12168"/>
+    <workbookView xWindow="192" yWindow="72" windowWidth="15300" windowHeight="12168" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="4" r:id="rId1"/>
     <sheet name="small_deform2" sheetId="1" r:id="rId2"/>
+    <sheet name="Chart1_harden" sheetId="6" r:id="rId3"/>
+    <sheet name="small_deform_harden2" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="small_deform2" localSheetId="3">small_deform_harden2!$C$3:$H$24</definedName>
     <definedName name="small_deform2" localSheetId="1">small_deform2!$C$3:$G$24</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -30,11 +33,22 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="small_deform21" type="6" refreshedVersion="3" background="1" saveData="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\tensor_mechanics\tests\weak_plane_shear\small_deform_harden2.csv" tab="0" comma="1">
+      <textFields count="5">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>time</t>
   </si>
@@ -67,6 +81,18 @@
   </si>
   <si>
     <t>sqrt(s_xz^2+s_yz^2)</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>residual</t>
+  </si>
+  <si>
+    <t>smoother</t>
+  </si>
+  <si>
+    <t>friction</t>
   </si>
 </sst>
 </file>
@@ -760,11 +786,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="122059776"/>
-        <c:axId val="123952512"/>
+        <c:axId val="192924288"/>
+        <c:axId val="203703040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="122059776"/>
+        <c:axId val="192924288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -791,12 +817,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123952512"/>
+        <c:crossAx val="203703040"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="123952512"/>
+        <c:axId val="203703040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3000"/>
@@ -828,7 +854,1483 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122059776"/>
+        <c:crossAx val="192924288"/>
+        <c:crossesAt val="-2000"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-AU"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Weak-plane shear yield function with and without hardening</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU" sz="1200" baseline="0"/>
+              <a:t>(Cohesion = (1000, 700), smoother = 500, friction_angle = (45, 30))</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>no hardening</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>small_deform2!$O$9:$O$360</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="352"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-200</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-300</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-400</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-500</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-600</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-700</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-800</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-900</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-1100</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-1200</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-1300</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-1400</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-1500</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-1600</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-1700</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-1800</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-1900</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-2000</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-2100</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-2200</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-2300</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-2400</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-2500</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-2600</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-2700</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-2800</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-2900</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-3000</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-3100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>small_deform2!$P$9:$P$360</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="352"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100.4987562112089</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>142.82856857085699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>175.78395831246945</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>203.96078054371139</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>229.128784747792</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>252.19040425836982</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>273.67864366808016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>293.9387691339814</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>313.20919526731649</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>331.66247903554</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>349.42810419312298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>366.60605559646717</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>383.27535793473601</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>399.49968710876357</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>415.33119314590374</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>430.81318457076031</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>445.98206241955518</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>460.86874487211651</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>475.49973711874964</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>489.89794855663564</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>504.0833264451424</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>518.0733538795447</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>531.88344587888798</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>545.52726787943425</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>559.01699437494744</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>572.36352085016733</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>585.57663887829403</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>598.66518188383066</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>611.63714733492111</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>624.49979983983985</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>748.33147735478826</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>866.02540378443859</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>979.79589711327128</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1090.8712114635714</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1307.669683062202</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1414.2135623730951</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1519.8684153570664</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1624.807680927192</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1729.1616465790582</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1833.030277982336</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1936.4916731037085</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2039.6078054371139</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2142.4285285628548</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2244.9944320643649</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2347.3389188611004</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2449.4897427831779</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2551.4701644346146</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2653.29983228432</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2754.995462791182</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2856.5713714171402</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2958.0398915498081</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3059.411708155671</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3160.6961258558217</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3261.9012860600183</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3363.0343441600476</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3464.1016151377544</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3565.1086939951774</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3666.0605559646719</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3766.9616403674727</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3867.8159211627431</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3968.6269665968857</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4069.3979898751609</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>MOOSE no hardening</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>small_deform2!$G$7:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>389.93270675526998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>189.63413986908</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-14.134943721578001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-218.89946991216999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-424.10001865372999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-629.53356129248004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-835.10731991662999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1040.7724678059999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1246.5007071236</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1452.2744416769999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1658.0821251371001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>small_deform2!$I$7:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>4.8196077420862001E-15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6214664036657999E-14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0719255144604003E-14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8011407739756E-13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8024462619458E-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.5354888966448995E-12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0375987821129997E-11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>349.54260744201702</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>637.72428200299692</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>882.30870299539026</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1111.6268589876461</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1333.4385950731812</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1550.9275923690814</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1765.6768298948614</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1978.5719487594361</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2190.1504271310123</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2400.7586415853084</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2610.6304275977122</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>With hardening</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:prstClr val="black"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>small_deform_harden2!$P$4:$P$720</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="717"/>
+                <c:pt idx="0">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-80</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-200</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-300</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-400</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-500</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-600</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-700</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-800</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-900</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-1000</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-1100</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-1200</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-1300</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-1400</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>-1500</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>-1600</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>-1700</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-1800</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>-1900</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>-2000</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>-2100</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>-2200</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>-2300</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>-2400</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>-2500</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>-2600</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>-2700</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>-2800</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>-2900</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>-3000</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>-3100</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>-3200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>small_deform_harden2!$Q$4:$Q$720</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="717"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>60.947561059254213</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>97.796603388834086</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>124.42030676855364</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>146.50363990370934</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>165.87009055389467</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>183.38245292924077</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>199.52951613984334</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>214.61965950565067</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>228.86204435928121</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>242.40614496535437</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>255.36309355951542</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>267.81812234102796</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>279.83825761130055</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>291.47730762145119</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>302.7792231317037</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>313.78043554194522</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>324.51152855363136</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>334.99846158781446</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>345.2634834946453</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>355.32582719270283</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>365.2022461214699</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>374.90743436323248</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>384.45435980899333</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>393.85453136676097</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>403.11821547380578</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>412.25461317262068</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>421.27200617189754</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>430.17787826985023</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>438.9790170248134</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>447.68159945441079</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>456.29126471883535</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>464.81317611921867</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>473.25207426489294</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>481.61232289537458</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>489.89794855663564</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>498.11267510673537</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>506.25995384845805</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>514.34298994539063</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>522.36476566471481</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>530.32806089873009</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>538.23547134309968</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>546.08942464940355</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>553.89219482004921</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>561.64591507273758</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>569.35258936785476</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>644.19826816472323</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>715.88205247767087</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>785.27032548003729</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>852.92351460495638</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>919.22479629266172</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>984.44735620507731</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1048.7924650881671</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1112.4123961817975</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1175.4249062355318</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1237.9227552175284</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1299.9801737867278</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1361.6573810097946</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1423.0038162088672</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1484.0604992041983</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1544.8617855064235</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1605.4366926181306</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1665.809916634505</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1726.0026214863456</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1786.0330587825872</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1845.9170597341308</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1905.6684293017452</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1965.2992647746878</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2024.8202153468199</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2084.2406951926218</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2143.5690595788074</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2202.8127513560439</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2261.9784235391517</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2321.0720424500428</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2380.098974958064</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2439.0640626306449</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2497.9716850482628</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>MOOSE with hardening</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>small_deform_harden2!$H$7:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>606.36034689370001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>346.41100614302002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>346.41016151378</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>346.41016151378</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>346.41016151378</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>346.41016151378</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>346.41016151378</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>198.62341046217</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-10.960827783213</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-222.34462695530999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-434.12224506963997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-646.01581593645005</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-857.94373824307002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1069.8779240179001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1281.8080699151999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1493.7305693430999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-1705.6445077778999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-1917.5500704643</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>small_deform_harden2!$J$7:$J$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2.6172177466328998E-15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5096207568403001E-14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0464012671553999E-13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4373907466883002E-13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5664483152639999E-12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2124977999059E-11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.7327180138445999E-11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>304.3096328546668</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>498.8981252225766</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>660.4526141395105</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>808.52847279864841</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>949.35782063278054</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1085.7359889601644</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1219.1460018942225</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1350.4624026077672</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1480.2396957595722</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1608.8488131546021</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1736.5483842074702</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="50892800"/>
+        <c:axId val="50894336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="50892800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="600"/>
+          <c:min val="-2000"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Normal stress (Pa)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50894336"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="500"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="50894336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3000"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Shear</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> stress (Pa)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50892800"/>
         <c:crossesAt val="-2000"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -846,7 +2348,18 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -880,8 +2393,39 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9272016" cy="6041136"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="small_deform2" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="small_deform2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2371,4 +3915,1619 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C1:U105"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P75" sqref="P75:Q105"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:21">
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1">
+        <f>30*PI()/180</f>
+        <v>0.52359877559829882</v>
+      </c>
+      <c r="R1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1">
+        <v>500</v>
+      </c>
+      <c r="T1" t="s">
+        <v>12</v>
+      </c>
+      <c r="U1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="2" spans="3:21">
+      <c r="M2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="3:21">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3">
+        <f>TAN(Q1)</f>
+        <v>0.57735026918962573</v>
+      </c>
+    </row>
+    <row r="4" spans="3:21">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>SQRT(G4*G4+F4*F4)</f>
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1000</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>600</v>
+      </c>
+      <c r="Q4" t="e">
+        <f>SQRT(($U$1-P4*TAN($Q$1))^2-($S$1)^2)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="3:21">
+      <c r="C5" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-300.00000986725001</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4.6528904803216999E-16</v>
+      </c>
+      <c r="H5">
+        <v>199.99999013275999</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5">
+        <f t="shared" ref="J5:J24" si="0">SQRT(G5*G5+F5*F5)</f>
+        <v>4.6528904803216999E-16</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5">
+        <v>-2000</v>
+      </c>
+      <c r="N5">
+        <v>3000</v>
+      </c>
+      <c r="P5">
+        <f>P4-10</f>
+        <v>590</v>
+      </c>
+      <c r="Q5" t="e">
+        <f t="shared" ref="Q5:Q68" si="1">SQRT(($U$1-P5*TAN($Q$1))^2-($S$1)^2)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="6" spans="3:21">
+      <c r="C6" s="1">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="D6">
+        <v>-100.00003971851</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>9.3057800300654E-16</v>
+      </c>
+      <c r="H6">
+        <v>399.99996028149002</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>9.3057800300654E-16</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="P6">
+        <f t="shared" ref="P6:P69" si="2">P5-10</f>
+        <v>580</v>
+      </c>
+      <c r="Q6" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21">
+      <c r="C7" s="1">
+        <v>2.9999999999999999E-7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-5.1664337729561999E-4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-1.2333367632570999E-8</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2.6172177466328998E-15</v>
+      </c>
+      <c r="H7">
+        <v>606.36034689370001</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>2.6172177466328998E-15</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>570</v>
+      </c>
+      <c r="Q7" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="3:21">
+      <c r="C8" s="1">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4.8764692189707002E-4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.3162914037801001E-5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>-1.5096207568403001E-14</v>
+      </c>
+      <c r="H8">
+        <v>346.41100614302002</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>1.5096207568403001E-14</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>560</v>
+      </c>
+      <c r="Q8" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="3:21">
+      <c r="C9" s="1">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.8891931822851E-5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1.0464012671553999E-13</v>
+      </c>
+      <c r="H9">
+        <v>346.41016151378</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>1.0464012671553999E-13</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>550</v>
+      </c>
+      <c r="Q9" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="3:21">
+      <c r="C10" s="1">
+        <v>5.9999999999999997E-7</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.4620924841071E-5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>-5.4373907466883002E-13</v>
+      </c>
+      <c r="H10">
+        <v>346.41016151378</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>5.4373907466883002E-13</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>540</v>
+      </c>
+      <c r="Q10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="3:21">
+      <c r="C11" s="1">
+        <v>6.9999999999999997E-7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3.0349917286849001E-5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2.5664483152639999E-12</v>
+      </c>
+      <c r="H11">
+        <v>346.41016151378</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>2.5664483152639999E-12</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="P11">
+        <f t="shared" si="2"/>
+        <v>530</v>
+      </c>
+      <c r="Q11" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21">
+      <c r="C12" s="1">
+        <v>7.9999999999999996E-7</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3.6078909147465003E-5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>-1.2124977999059E-11</v>
+      </c>
+      <c r="H12">
+        <v>346.41016151378</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>1.2124977999059E-11</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="P12">
+        <f t="shared" si="2"/>
+        <v>520</v>
+      </c>
+      <c r="Q12" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="13" spans="3:21">
+      <c r="C13" s="1">
+        <v>8.9999999999999996E-7</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-1.1368683772161999E-13</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4.1807900435639002E-5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>5.7327180138445999E-11</v>
+      </c>
+      <c r="H13">
+        <v>346.41016151378</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>5.7327180138445999E-11</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="P13">
+        <f t="shared" si="2"/>
+        <v>510</v>
+      </c>
+      <c r="Q13" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21">
+      <c r="C14" s="1">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.9021840023801999E-4</v>
+      </c>
+      <c r="E14" s="1">
+        <v>5.1770429264238E-5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>157.72420493230999</v>
+      </c>
+      <c r="G14">
+        <v>260.24493813830998</v>
+      </c>
+      <c r="H14">
+        <v>198.62341046217</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>304.3096328546668</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="P14">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="Q14" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21">
+      <c r="C15" s="1">
+        <v>1.1000000000000001E-6</v>
+      </c>
+      <c r="D15" s="1">
+        <v>7.7506001616711997E-10</v>
+      </c>
+      <c r="E15" s="1">
+        <v>5.2044969121864998E-5</v>
+      </c>
+      <c r="F15">
+        <v>257.65133149913999</v>
+      </c>
+      <c r="G15">
+        <v>427.21789607567001</v>
+      </c>
+      <c r="H15">
+        <v>-10.960827783213</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>498.8981252225766</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="2"/>
+        <v>490</v>
+      </c>
+      <c r="Q15" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21">
+      <c r="C16" s="1">
+        <v>1.1999999999999999E-6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2.7141311420564002E-10</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5.2371054096859998E-5</v>
+      </c>
+      <c r="F16">
+        <v>340.61105326081997</v>
+      </c>
+      <c r="G16">
+        <v>565.84606203477995</v>
+      </c>
+      <c r="H16">
+        <v>-222.34462695530999</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>660.4526141395105</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="2"/>
+        <v>480</v>
+      </c>
+      <c r="Q16" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17">
+      <c r="C17" s="1">
+        <v>1.3E-6</v>
+      </c>
+      <c r="D17" s="1">
+        <v>7.2067465171698998E-4</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5.2708416962179997E-5</v>
+      </c>
+      <c r="F17">
+        <v>416.67332486516</v>
+      </c>
+      <c r="G17">
+        <v>692.89366548693999</v>
+      </c>
+      <c r="H17">
+        <v>-434.12224506963997</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>808.52847279864841</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="2"/>
+        <v>470</v>
+      </c>
+      <c r="Q17" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17">
+      <c r="C18" s="1">
+        <v>1.3999999999999999E-6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2.9083095097349001E-4</v>
+      </c>
+      <c r="E18" s="1">
+        <v>5.3049098367189001E-5</v>
+      </c>
+      <c r="F18">
+        <v>489.03509539286</v>
+      </c>
+      <c r="G18">
+        <v>813.71060400532997</v>
+      </c>
+      <c r="H18">
+        <v>-646.01581593645005</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>949.35782063278054</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="2"/>
+        <v>460</v>
+      </c>
+      <c r="Q18" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="19" spans="3:17">
+      <c r="C19" s="1">
+        <v>1.5E-6</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1.2392816188367E-4</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5.3390760918198E-5</v>
+      </c>
+      <c r="F19">
+        <v>559.12676832838997</v>
+      </c>
+      <c r="G19">
+        <v>930.69860570539004</v>
+      </c>
+      <c r="H19">
+        <v>-857.94373824307002</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>1085.7359889601644</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="2"/>
+        <v>450</v>
+      </c>
+      <c r="Q19" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17">
+      <c r="C20" s="1">
+        <v>1.5999999999999999E-6</v>
+      </c>
+      <c r="D20" s="1">
+        <v>5.6158186097832003E-5</v>
+      </c>
+      <c r="E20" s="1">
+        <v>5.3732600085378002E-5</v>
+      </c>
+      <c r="F20">
+        <v>627.70594040114997</v>
+      </c>
+      <c r="G20">
+        <v>1045.1326357548</v>
+      </c>
+      <c r="H20">
+        <v>-1069.8779240179001</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>1219.1460018942225</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="2"/>
+        <v>440</v>
+      </c>
+      <c r="Q20" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17">
+      <c r="C21" s="1">
+        <v>1.7E-6</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2.6962447066125999E-5</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5.4074320764552998E-5</v>
+      </c>
+      <c r="F21">
+        <v>695.21883930039996</v>
+      </c>
+      <c r="G21">
+        <v>1157.7648579651</v>
+      </c>
+      <c r="H21">
+        <v>-1281.8080699151999</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>1350.4624026077672</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="2"/>
+        <v>430</v>
+      </c>
+      <c r="Q21" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17">
+      <c r="C22" s="1">
+        <v>1.7999999999999999E-6</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.3634324346867E-5</v>
+      </c>
+      <c r="E22" s="1">
+        <v>5.4415819670677998E-5</v>
+      </c>
+      <c r="F22">
+        <v>761.94815574426002</v>
+      </c>
+      <c r="G22">
+        <v>1269.0723245191</v>
+      </c>
+      <c r="H22">
+        <v>-1493.7305693430999</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>1480.2396957595722</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="2"/>
+        <v>420</v>
+      </c>
+      <c r="Q22" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17">
+      <c r="C23" s="1">
+        <v>1.9E-6</v>
+      </c>
+      <c r="D23" s="1">
+        <v>7.2188567230568997E-6</v>
+      </c>
+      <c r="E23" s="1">
+        <v>5.4757070626749997E-5</v>
+      </c>
+      <c r="F23">
+        <v>828.08287688804</v>
+      </c>
+      <c r="G23">
+        <v>1379.3742249997999</v>
+      </c>
+      <c r="H23">
+        <v>-1705.6445077778999</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>1608.8488131546021</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="2"/>
+        <v>410</v>
+      </c>
+      <c r="Q23" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17">
+      <c r="C24" s="1">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3.9806978406887001E-6</v>
+      </c>
+      <c r="E24" s="1">
+        <v>5.5098078954293E-5</v>
+      </c>
+      <c r="F24">
+        <v>893.75471301650998</v>
+      </c>
+      <c r="G24">
+        <v>1488.8931471581</v>
+      </c>
+      <c r="H24">
+        <v>-1917.5500704643</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>1736.5483842074702</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="2"/>
+        <v>400</v>
+      </c>
+      <c r="Q24" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17">
+      <c r="P25">
+        <f t="shared" si="2"/>
+        <v>390</v>
+      </c>
+      <c r="Q25" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17">
+      <c r="P26">
+        <f t="shared" si="2"/>
+        <v>380</v>
+      </c>
+      <c r="Q26" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17">
+      <c r="P27">
+        <f t="shared" si="2"/>
+        <v>370</v>
+      </c>
+      <c r="Q27" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17">
+      <c r="P28">
+        <f t="shared" si="2"/>
+        <v>360</v>
+      </c>
+      <c r="Q28" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17">
+      <c r="P29">
+        <f t="shared" si="2"/>
+        <v>350</v>
+      </c>
+      <c r="Q29" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17">
+      <c r="P30">
+        <f t="shared" si="2"/>
+        <v>340</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="1"/>
+        <v>60.947561059254213</v>
+      </c>
+    </row>
+    <row r="31" spans="3:17">
+      <c r="P31">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="1"/>
+        <v>97.796603388834086</v>
+      </c>
+    </row>
+    <row r="32" spans="3:17">
+      <c r="P32">
+        <f t="shared" si="2"/>
+        <v>320</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="1"/>
+        <v>124.42030676855364</v>
+      </c>
+    </row>
+    <row r="33" spans="16:17">
+      <c r="P33">
+        <f t="shared" si="2"/>
+        <v>310</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="1"/>
+        <v>146.50363990370934</v>
+      </c>
+    </row>
+    <row r="34" spans="16:17">
+      <c r="P34">
+        <f t="shared" si="2"/>
+        <v>300</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="1"/>
+        <v>165.87009055389467</v>
+      </c>
+    </row>
+    <row r="35" spans="16:17">
+      <c r="P35">
+        <f t="shared" si="2"/>
+        <v>290</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="1"/>
+        <v>183.38245292924077</v>
+      </c>
+    </row>
+    <row r="36" spans="16:17">
+      <c r="P36">
+        <f t="shared" si="2"/>
+        <v>280</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="1"/>
+        <v>199.52951613984334</v>
+      </c>
+    </row>
+    <row r="37" spans="16:17">
+      <c r="P37">
+        <f t="shared" si="2"/>
+        <v>270</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="1"/>
+        <v>214.61965950565067</v>
+      </c>
+    </row>
+    <row r="38" spans="16:17">
+      <c r="P38">
+        <f t="shared" si="2"/>
+        <v>260</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="1"/>
+        <v>228.86204435928121</v>
+      </c>
+    </row>
+    <row r="39" spans="16:17">
+      <c r="P39">
+        <f t="shared" si="2"/>
+        <v>250</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="1"/>
+        <v>242.40614496535437</v>
+      </c>
+    </row>
+    <row r="40" spans="16:17">
+      <c r="P40">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="1"/>
+        <v>255.36309355951542</v>
+      </c>
+    </row>
+    <row r="41" spans="16:17">
+      <c r="P41">
+        <f t="shared" si="2"/>
+        <v>230</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="1"/>
+        <v>267.81812234102796</v>
+      </c>
+    </row>
+    <row r="42" spans="16:17">
+      <c r="P42">
+        <f t="shared" si="2"/>
+        <v>220</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="1"/>
+        <v>279.83825761130055</v>
+      </c>
+    </row>
+    <row r="43" spans="16:17">
+      <c r="P43">
+        <f t="shared" si="2"/>
+        <v>210</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="1"/>
+        <v>291.47730762145119</v>
+      </c>
+    </row>
+    <row r="44" spans="16:17">
+      <c r="P44">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="1"/>
+        <v>302.7792231317037</v>
+      </c>
+    </row>
+    <row r="45" spans="16:17">
+      <c r="P45">
+        <f t="shared" si="2"/>
+        <v>190</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="1"/>
+        <v>313.78043554194522</v>
+      </c>
+    </row>
+    <row r="46" spans="16:17">
+      <c r="P46">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="1"/>
+        <v>324.51152855363136</v>
+      </c>
+    </row>
+    <row r="47" spans="16:17">
+      <c r="P47">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="1"/>
+        <v>334.99846158781446</v>
+      </c>
+    </row>
+    <row r="48" spans="16:17">
+      <c r="P48">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="1"/>
+        <v>345.2634834946453</v>
+      </c>
+    </row>
+    <row r="49" spans="16:17">
+      <c r="P49">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="1"/>
+        <v>355.32582719270283</v>
+      </c>
+    </row>
+    <row r="50" spans="16:17">
+      <c r="P50">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="1"/>
+        <v>365.2022461214699</v>
+      </c>
+    </row>
+    <row r="51" spans="16:17">
+      <c r="P51">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="1"/>
+        <v>374.90743436323248</v>
+      </c>
+    </row>
+    <row r="52" spans="16:17">
+      <c r="P52">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="1"/>
+        <v>384.45435980899333</v>
+      </c>
+    </row>
+    <row r="53" spans="16:17">
+      <c r="P53">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="1"/>
+        <v>393.85453136676097</v>
+      </c>
+    </row>
+    <row r="54" spans="16:17">
+      <c r="P54">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="1"/>
+        <v>403.11821547380578</v>
+      </c>
+    </row>
+    <row r="55" spans="16:17">
+      <c r="P55">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="1"/>
+        <v>412.25461317262068</v>
+      </c>
+    </row>
+    <row r="56" spans="16:17">
+      <c r="P56">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="1"/>
+        <v>421.27200617189754</v>
+      </c>
+    </row>
+    <row r="57" spans="16:17">
+      <c r="P57">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="1"/>
+        <v>430.17787826985023</v>
+      </c>
+    </row>
+    <row r="58" spans="16:17">
+      <c r="P58">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="1"/>
+        <v>438.9790170248134</v>
+      </c>
+    </row>
+    <row r="59" spans="16:17">
+      <c r="P59">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="1"/>
+        <v>447.68159945441079</v>
+      </c>
+    </row>
+    <row r="60" spans="16:17">
+      <c r="P60">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="1"/>
+        <v>456.29126471883535</v>
+      </c>
+    </row>
+    <row r="61" spans="16:17">
+      <c r="P61">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" si="1"/>
+        <v>464.81317611921867</v>
+      </c>
+    </row>
+    <row r="62" spans="16:17">
+      <c r="P62">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="1"/>
+        <v>473.25207426489294</v>
+      </c>
+    </row>
+    <row r="63" spans="16:17">
+      <c r="P63">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="1"/>
+        <v>481.61232289537458</v>
+      </c>
+    </row>
+    <row r="64" spans="16:17">
+      <c r="P64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q64">
+        <f t="shared" si="1"/>
+        <v>489.89794855663564</v>
+      </c>
+    </row>
+    <row r="65" spans="16:17">
+      <c r="P65">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="Q65">
+        <f t="shared" si="1"/>
+        <v>498.11267510673537</v>
+      </c>
+    </row>
+    <row r="66" spans="16:17">
+      <c r="P66">
+        <f t="shared" si="2"/>
+        <v>-20</v>
+      </c>
+      <c r="Q66">
+        <f t="shared" si="1"/>
+        <v>506.25995384845805</v>
+      </c>
+    </row>
+    <row r="67" spans="16:17">
+      <c r="P67">
+        <f t="shared" si="2"/>
+        <v>-30</v>
+      </c>
+      <c r="Q67">
+        <f t="shared" si="1"/>
+        <v>514.34298994539063</v>
+      </c>
+    </row>
+    <row r="68" spans="16:17">
+      <c r="P68">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
+      <c r="Q68">
+        <f t="shared" si="1"/>
+        <v>522.36476566471481</v>
+      </c>
+    </row>
+    <row r="69" spans="16:17">
+      <c r="P69">
+        <f t="shared" si="2"/>
+        <v>-50</v>
+      </c>
+      <c r="Q69">
+        <f t="shared" ref="Q69:Q105" si="3">SQRT(($U$1-P69*TAN($Q$1))^2-($S$1)^2)</f>
+        <v>530.32806089873009</v>
+      </c>
+    </row>
+    <row r="70" spans="16:17">
+      <c r="P70">
+        <f t="shared" ref="P70:P72" si="4">P69-10</f>
+        <v>-60</v>
+      </c>
+      <c r="Q70">
+        <f t="shared" si="3"/>
+        <v>538.23547134309968</v>
+      </c>
+    </row>
+    <row r="71" spans="16:17">
+      <c r="P71">
+        <f t="shared" si="4"/>
+        <v>-70</v>
+      </c>
+      <c r="Q71">
+        <f t="shared" si="3"/>
+        <v>546.08942464940355</v>
+      </c>
+    </row>
+    <row r="72" spans="16:17">
+      <c r="P72">
+        <f t="shared" si="4"/>
+        <v>-80</v>
+      </c>
+      <c r="Q72">
+        <f t="shared" si="3"/>
+        <v>553.89219482004921</v>
+      </c>
+    </row>
+    <row r="73" spans="16:17">
+      <c r="P73">
+        <f t="shared" ref="P73:P74" si="5">P72-10</f>
+        <v>-90</v>
+      </c>
+      <c r="Q73">
+        <f t="shared" si="3"/>
+        <v>561.64591507273758</v>
+      </c>
+    </row>
+    <row r="74" spans="16:17">
+      <c r="P74">
+        <f t="shared" si="5"/>
+        <v>-100</v>
+      </c>
+      <c r="Q74">
+        <f t="shared" si="3"/>
+        <v>569.35258936785476</v>
+      </c>
+    </row>
+    <row r="75" spans="16:17">
+      <c r="P75">
+        <f>P74-100</f>
+        <v>-200</v>
+      </c>
+      <c r="Q75">
+        <f t="shared" si="3"/>
+        <v>644.19826816472323</v>
+      </c>
+    </row>
+    <row r="76" spans="16:17">
+      <c r="P76">
+        <f t="shared" ref="P76:P105" si="6">P75-100</f>
+        <v>-300</v>
+      </c>
+      <c r="Q76">
+        <f t="shared" si="3"/>
+        <v>715.88205247767087</v>
+      </c>
+    </row>
+    <row r="77" spans="16:17">
+      <c r="P77">
+        <f t="shared" si="6"/>
+        <v>-400</v>
+      </c>
+      <c r="Q77">
+        <f t="shared" si="3"/>
+        <v>785.27032548003729</v>
+      </c>
+    </row>
+    <row r="78" spans="16:17">
+      <c r="P78">
+        <f t="shared" si="6"/>
+        <v>-500</v>
+      </c>
+      <c r="Q78">
+        <f t="shared" si="3"/>
+        <v>852.92351460495638</v>
+      </c>
+    </row>
+    <row r="79" spans="16:17">
+      <c r="P79">
+        <f t="shared" si="6"/>
+        <v>-600</v>
+      </c>
+      <c r="Q79">
+        <f t="shared" si="3"/>
+        <v>919.22479629266172</v>
+      </c>
+    </row>
+    <row r="80" spans="16:17">
+      <c r="P80">
+        <f t="shared" si="6"/>
+        <v>-700</v>
+      </c>
+      <c r="Q80">
+        <f t="shared" si="3"/>
+        <v>984.44735620507731</v>
+      </c>
+    </row>
+    <row r="81" spans="16:17">
+      <c r="P81">
+        <f t="shared" si="6"/>
+        <v>-800</v>
+      </c>
+      <c r="Q81">
+        <f t="shared" si="3"/>
+        <v>1048.7924650881671</v>
+      </c>
+    </row>
+    <row r="82" spans="16:17">
+      <c r="P82">
+        <f t="shared" si="6"/>
+        <v>-900</v>
+      </c>
+      <c r="Q82">
+        <f t="shared" si="3"/>
+        <v>1112.4123961817975</v>
+      </c>
+    </row>
+    <row r="83" spans="16:17">
+      <c r="P83">
+        <f t="shared" si="6"/>
+        <v>-1000</v>
+      </c>
+      <c r="Q83">
+        <f t="shared" si="3"/>
+        <v>1175.4249062355318</v>
+      </c>
+    </row>
+    <row r="84" spans="16:17">
+      <c r="P84">
+        <f t="shared" si="6"/>
+        <v>-1100</v>
+      </c>
+      <c r="Q84">
+        <f t="shared" si="3"/>
+        <v>1237.9227552175284</v>
+      </c>
+    </row>
+    <row r="85" spans="16:17">
+      <c r="P85">
+        <f t="shared" si="6"/>
+        <v>-1200</v>
+      </c>
+      <c r="Q85">
+        <f t="shared" si="3"/>
+        <v>1299.9801737867278</v>
+      </c>
+    </row>
+    <row r="86" spans="16:17">
+      <c r="P86">
+        <f t="shared" si="6"/>
+        <v>-1300</v>
+      </c>
+      <c r="Q86">
+        <f t="shared" si="3"/>
+        <v>1361.6573810097946</v>
+      </c>
+    </row>
+    <row r="87" spans="16:17">
+      <c r="P87">
+        <f t="shared" si="6"/>
+        <v>-1400</v>
+      </c>
+      <c r="Q87">
+        <f t="shared" si="3"/>
+        <v>1423.0038162088672</v>
+      </c>
+    </row>
+    <row r="88" spans="16:17">
+      <c r="P88">
+        <f t="shared" si="6"/>
+        <v>-1500</v>
+      </c>
+      <c r="Q88">
+        <f t="shared" si="3"/>
+        <v>1484.0604992041983</v>
+      </c>
+    </row>
+    <row r="89" spans="16:17">
+      <c r="P89">
+        <f t="shared" si="6"/>
+        <v>-1600</v>
+      </c>
+      <c r="Q89">
+        <f t="shared" si="3"/>
+        <v>1544.8617855064235</v>
+      </c>
+    </row>
+    <row r="90" spans="16:17">
+      <c r="P90">
+        <f t="shared" si="6"/>
+        <v>-1700</v>
+      </c>
+      <c r="Q90">
+        <f t="shared" si="3"/>
+        <v>1605.4366926181306</v>
+      </c>
+    </row>
+    <row r="91" spans="16:17">
+      <c r="P91">
+        <f t="shared" si="6"/>
+        <v>-1800</v>
+      </c>
+      <c r="Q91">
+        <f t="shared" si="3"/>
+        <v>1665.809916634505</v>
+      </c>
+    </row>
+    <row r="92" spans="16:17">
+      <c r="P92">
+        <f t="shared" si="6"/>
+        <v>-1900</v>
+      </c>
+      <c r="Q92">
+        <f t="shared" si="3"/>
+        <v>1726.0026214863456</v>
+      </c>
+    </row>
+    <row r="93" spans="16:17">
+      <c r="P93">
+        <f t="shared" si="6"/>
+        <v>-2000</v>
+      </c>
+      <c r="Q93">
+        <f t="shared" si="3"/>
+        <v>1786.0330587825872</v>
+      </c>
+    </row>
+    <row r="94" spans="16:17">
+      <c r="P94">
+        <f t="shared" si="6"/>
+        <v>-2100</v>
+      </c>
+      <c r="Q94">
+        <f t="shared" si="3"/>
+        <v>1845.9170597341308</v>
+      </c>
+    </row>
+    <row r="95" spans="16:17">
+      <c r="P95">
+        <f t="shared" si="6"/>
+        <v>-2200</v>
+      </c>
+      <c r="Q95">
+        <f t="shared" si="3"/>
+        <v>1905.6684293017452</v>
+      </c>
+    </row>
+    <row r="96" spans="16:17">
+      <c r="P96">
+        <f t="shared" si="6"/>
+        <v>-2300</v>
+      </c>
+      <c r="Q96">
+        <f t="shared" si="3"/>
+        <v>1965.2992647746878</v>
+      </c>
+    </row>
+    <row r="97" spans="16:17">
+      <c r="P97">
+        <f t="shared" si="6"/>
+        <v>-2400</v>
+      </c>
+      <c r="Q97">
+        <f t="shared" si="3"/>
+        <v>2024.8202153468199</v>
+      </c>
+    </row>
+    <row r="98" spans="16:17">
+      <c r="P98">
+        <f t="shared" si="6"/>
+        <v>-2500</v>
+      </c>
+      <c r="Q98">
+        <f t="shared" si="3"/>
+        <v>2084.2406951926218</v>
+      </c>
+    </row>
+    <row r="99" spans="16:17">
+      <c r="P99">
+        <f t="shared" si="6"/>
+        <v>-2600</v>
+      </c>
+      <c r="Q99">
+        <f t="shared" si="3"/>
+        <v>2143.5690595788074</v>
+      </c>
+    </row>
+    <row r="100" spans="16:17">
+      <c r="P100">
+        <f t="shared" si="6"/>
+        <v>-2700</v>
+      </c>
+      <c r="Q100">
+        <f t="shared" si="3"/>
+        <v>2202.8127513560439</v>
+      </c>
+    </row>
+    <row r="101" spans="16:17">
+      <c r="P101">
+        <f t="shared" si="6"/>
+        <v>-2800</v>
+      </c>
+      <c r="Q101">
+        <f t="shared" si="3"/>
+        <v>2261.9784235391517</v>
+      </c>
+    </row>
+    <row r="102" spans="16:17">
+      <c r="P102">
+        <f t="shared" si="6"/>
+        <v>-2900</v>
+      </c>
+      <c r="Q102">
+        <f t="shared" si="3"/>
+        <v>2321.0720424500428</v>
+      </c>
+    </row>
+    <row r="103" spans="16:17">
+      <c r="P103">
+        <f t="shared" si="6"/>
+        <v>-3000</v>
+      </c>
+      <c r="Q103">
+        <f t="shared" si="3"/>
+        <v>2380.098974958064</v>
+      </c>
+    </row>
+    <row r="104" spans="16:17">
+      <c r="P104">
+        <f t="shared" si="6"/>
+        <v>-3100</v>
+      </c>
+      <c r="Q104">
+        <f t="shared" si="3"/>
+        <v>2439.0640626306449</v>
+      </c>
+    </row>
+    <row r="105" spans="16:17">
+      <c r="P105">
+        <f t="shared" si="6"/>
+        <v>-3200</v>
+      </c>
+      <c r="Q105">
+        <f t="shared" si="3"/>
+        <v>2497.9716850482628</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>